<commit_message>
Modified SSAS for VM
</commit_message>
<xml_diff>
--- a/DS2_Cube/SSAS Cube - Location Analysis.xlsx
+++ b/DS2_Cube/SSAS Cube - Location Analysis.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Oleh\EPAM\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleh_Kushnir\Desktop\DS2-Project\DS2_Cube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40E74B43-669E-4D02-ADEA-C0C5FFDCAD1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3A71F2-0171-4218-8915-3DF7CFD194C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{8B9F041E-8F88-4BD4-BD77-675DFDB5A86F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8B9F041E-8F88-4BD4-BD77-675DFDB5A86F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Location Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Locations Overview" sheetId="5" r:id="rId1"/>
     <sheet name="Cities with Total more 1k" sheetId="2" r:id="rId2"/>
     <sheet name="City with max Total" sheetId="3" r:id="rId3"/>
     <sheet name="Count cities" sheetId="4" r:id="rId4"/>
@@ -22,26 +22,12 @@
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Cities with Total more 1k'!$A$1:$F$48</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">'City with max Total'!$A$1:$A$2</definedName>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Count cities'!$A$1:$H$62</definedName>
-    <definedName name="Slicer_Region_Country_State_City">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="92" r:id="rId5"/>
+    <pivotCache cacheId="57" r:id="rId5"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
-      <x14:pivotCaches>
-        <pivotCache cacheId="59" r:id="rId6"/>
-      </x14:pivotCaches>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
-      <x14:slicerCaches>
-        <x14:slicerCache r:id="rId7"/>
-      </x14:slicerCaches>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -55,20 +41,24 @@
     <dbPr connection="Provider=MSOLAP.8;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=DS2_SSAS;Data Source=DESKTOP-0OE0JIH\DAMSKIYSQL;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" command="DS2 Cube" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
   </connection>
-  <connection id="2" xr16:uid="{3734B2E5-970B-4014-B2CF-B1BBF936100E}" keepAlive="1" name="Query - Query1" description="Connection to the 'Query1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{06D46B2C-8A60-42ED-9657-EB10843D84AE}" odcFile="C:\Users\Oleh_Kushnir\Documents\My Data Sources\DS2 Cube.odc" keepAlive="1" name="DS2 Cube1" type="5" refreshedVersion="6" background="1">
+    <dbPr connection="Provider=MSOLAP.8;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=DS2_SSAS;Data Source=ECSD00300f36;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" command="DS2 Cube" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+  </connection>
+  <connection id="3" xr16:uid="{3734B2E5-970B-4014-B2CF-B1BBF936100E}" keepAlive="1" name="Query - Query1" description="Connection to the 'Query1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Query1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Query1]"/>
   </connection>
-  <connection id="3" xr16:uid="{C23078CB-3752-4A60-97CE-BEECF7EA1017}" keepAlive="1" name="Query - Query2" description="Connection to the 'Query2' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{C23078CB-3752-4A60-97CE-BEECF7EA1017}" keepAlive="1" name="Query - Query2" description="Connection to the 'Query2' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Query2;Extended Properties=&quot;&quot;" command="SELECT * FROM [Query2]"/>
   </connection>
-  <connection id="4" xr16:uid="{AC310123-12BA-401F-BD0C-3B8C40C34F59}" keepAlive="1" name="Query - Query3" description="Connection to the 'Query3' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="5" xr16:uid="{AC310123-12BA-401F-BD0C-3B8C40C34F59}" keepAlive="1" name="Query - Query3" description="Connection to the 'Query3' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Query3;Extended Properties=&quot;&quot;" command="SELECT * FROM [Query3]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="125">
   <si>
     <t>Australia</t>
   </si>
@@ -443,9 +433,6 @@
   </si>
   <si>
     <t>Quantity</t>
-  </si>
-  <si>
-    <t>Fact Order Count</t>
   </si>
 </sst>
 </file>
@@ -529,171 +516,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Region">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E465D57E-8599-4D7A-88E1-FBD0B4CCDC22}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7315200" y="85726"/>
-              <a:ext cx="1828800" cy="990600"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="uk-UA" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Country">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C3D5A3F-FB52-47E5-8B0C-BE3270966F02}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Country"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7305675" y="1152525"/>
-              <a:ext cx="1828800" cy="3409950"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="uk-UA" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Oleg" refreshedDate="44172.584971412034" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{6CE6FCBB-3CBB-4AC6-BC77-C9D2D455B508}">
-  <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="9">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Oleh Kushnir" refreshedDate="44173.788292824072" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{8780DD4C-5FA0-484E-90A6-358BB0ADAED3}">
+  <cacheSource type="external" connectionId="2"/>
+  <cacheFields count="8">
+    <cacheField name="[Measures].[Net Amount]" caption="Net Amount" numFmtId="0" hierarchy="23" level="32767"/>
+    <cacheField name="[Measures].[Quantity]" caption="Quantity" numFmtId="0" hierarchy="22" level="32767"/>
+    <cacheField name="[Measures].[Tax]" caption="Tax" numFmtId="0" hierarchy="24" level="32767"/>
+    <cacheField name="[Measures].[Total Amount]" caption="Total Amount" numFmtId="0" hierarchy="25" level="32767"/>
     <cacheField name="[Location].[Region-Country-State-City].[Region]" caption="Region" numFmtId="0" hierarchy="14" level="1">
       <sharedItems count="2">
         <s v="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]" c="Non-USA"/>
@@ -709,68 +539,59 @@
     <cacheField name="[Location].[Region-Country-State-City].[City]" caption="City" numFmtId="0" hierarchy="14" level="4">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
-    <cacheField name="[Measures].[Quantity]" caption="Quantity" numFmtId="0" hierarchy="22" level="32767"/>
-    <cacheField name="[Measures].[Net Amount]" caption="Net Amount" numFmtId="0" hierarchy="23" level="32767"/>
-    <cacheField name="[Measures].[Tax]" caption="Tax" numFmtId="0" hierarchy="24" level="32767"/>
-    <cacheField name="[Measures].[Total Amount]" caption="Total Amount" numFmtId="0" hierarchy="25" level="32767"/>
-    <cacheField name="[Measures].[Fact Order Count]" caption="Fact Order Count" numFmtId="0" hierarchy="26" level="32767"/>
   </cacheFields>
   <cacheHierarchies count="27">
-    <cacheHierarchy uniqueName="[Customer].[Age]" caption="Age" attribute="1" defaultMemberUniqueName="[Customer].[Age].[All]" allUniqueName="[Customer].[Age].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Customer ID]" caption="Customer ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Customer].[Customer ID].[All]" allUniqueName="[Customer].[Customer ID].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Full Name]" caption="Full Name" attribute="1" defaultMemberUniqueName="[Customer].[Full Name].[All]" allUniqueName="[Customer].[Full Name].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[Customer].[Gender].[All]" allUniqueName="[Customer].[Gender].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Gender-Age-Name]" caption="Gender-Age-Name" defaultMemberUniqueName="[Customer].[Gender-Age-Name].[All]" allUniqueName="[Customer].[Gender-Age-Name].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="4" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[Date ID]" caption="Date ID" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Date].[Date ID].[All]" allUniqueName="[Date].[Date ID].[All]" dimensionUniqueName="[Date]" displayFolder="" count="2" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[The Day]" caption="The Day" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Day].[All]" allUniqueName="[Date].[The Day].[All]" dimensionUniqueName="[Date]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[The Month]" caption="The Month" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Month].[All]" allUniqueName="[Date].[The Month].[All]" dimensionUniqueName="[Date]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[The Year]" caption="The Year" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Year].[All]" allUniqueName="[Date].[The Year].[All]" dimensionUniqueName="[Date]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[Year-Month-Day]" caption="Year-Month-Day" time="1" defaultMemberUniqueName="[Date].[Year-Month-Day].[All]" allUniqueName="[Date].[Year-Month-Day].[All]" dimensionUniqueName="[Date]" displayFolder="" count="4" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[City]" caption="City" attribute="1" defaultMemberUniqueName="[Location].[City].[All]" allUniqueName="[Location].[City].[All]" dimensionUniqueName="[Location]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Location].[Country].[All]" allUniqueName="[Location].[Country].[All]" dimensionUniqueName="[Location]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Location ID]" caption="Location ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Location].[Location ID].[All]" allUniqueName="[Location].[Location ID].[All]" dimensionUniqueName="[Location]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Region]" caption="Region" attribute="1" defaultMemberUniqueName="[Location].[Region].[All]" allUniqueName="[Location].[Region].[All]" dimensionUniqueName="[Location]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Customer].[Age]" caption="Age" attribute="1" defaultMemberUniqueName="[Customer].[Age].[All]" allUniqueName="[Customer].[Age].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Customer].[Customer ID]" caption="Customer ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Customer].[Customer ID].[All]" allUniqueName="[Customer].[Customer ID].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Customer].[Full Name]" caption="Full Name" attribute="1" defaultMemberUniqueName="[Customer].[Full Name].[All]" allUniqueName="[Customer].[Full Name].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Customer].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[Customer].[Gender].[All]" allUniqueName="[Customer].[Gender].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Customer].[Gender-Age-Name]" caption="Gender-Age-Name" defaultMemberUniqueName="[Customer].[Gender-Age-Name].[All]" allUniqueName="[Customer].[Gender-Age-Name].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Date].[Date ID]" caption="Date ID" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Date].[Date ID].[All]" allUniqueName="[Date].[Date ID].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Date].[The Day]" caption="The Day" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Day].[All]" allUniqueName="[Date].[The Day].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Date].[The Month]" caption="The Month" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Month].[All]" allUniqueName="[Date].[The Month].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Date].[The Year]" caption="The Year" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Year].[All]" allUniqueName="[Date].[The Year].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Date].[Year-Month-Day]" caption="Year-Month-Day" time="1" defaultMemberUniqueName="[Date].[Year-Month-Day].[All]" allUniqueName="[Date].[Year-Month-Day].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Location].[City]" caption="City" attribute="1" defaultMemberUniqueName="[Location].[City].[All]" allUniqueName="[Location].[City].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Location].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Location].[Country].[All]" allUniqueName="[Location].[Country].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Location].[Location ID]" caption="Location ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Location].[Location ID].[All]" allUniqueName="[Location].[Location ID].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Location].[Region]" caption="Region" attribute="1" defaultMemberUniqueName="[Location].[Region].[All]" allUniqueName="[Location].[Region].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Location].[Region-Country-State-City]" caption="Region-Country-State-City" defaultMemberUniqueName="[Location].[Region-Country-State-City].[All]" allUniqueName="[Location].[Region-Country-State-City].[All]" dimensionUniqueName="[Location]" displayFolder="" count="5" unbalanced="0">
       <fieldsUsage count="5">
         <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
-        <fieldUsage x="1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
+        <fieldUsage x="4"/>
+        <fieldUsage x="5"/>
+        <fieldUsage x="6"/>
+        <fieldUsage x="7"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Location].[State]" caption="State" attribute="1" defaultMemberUniqueName="[Location].[State].[All]" allUniqueName="[Location].[State].[All]" dimensionUniqueName="[Location]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Category]" caption="Category" attribute="1" defaultMemberUniqueName="[Product].[Category].[All]" allUniqueName="[Product].[Category].[All]" dimensionUniqueName="[Product]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[ID]" caption="ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Product].[ID].[All]" allUniqueName="[Product].[ID].[All]" dimensionUniqueName="[Product]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Price]" caption="Price" attribute="1" defaultMemberUniqueName="[Product].[Price].[All]" allUniqueName="[Product].[Price].[All]" dimensionUniqueName="[Product]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Special]" caption="Special" attribute="1" defaultMemberUniqueName="[Product].[Special].[All]" allUniqueName="[Product].[Special].[All]" dimensionUniqueName="[Product]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Special-Category-Title]" caption="Special-Category-Title" defaultMemberUniqueName="[Product].[Special-Category-Title].[All]" allUniqueName="[Product].[Special-Category-Title].[All]" dimensionUniqueName="[Product]" displayFolder="" count="4" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Title]" caption="Title" attribute="1" defaultMemberUniqueName="[Product].[Title].[All]" allUniqueName="[Product].[Title].[All]" dimensionUniqueName="[Product]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Location].[State]" caption="State" attribute="1" defaultMemberUniqueName="[Location].[State].[All]" allUniqueName="[Location].[State].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product].[Category]" caption="Category" attribute="1" defaultMemberUniqueName="[Product].[Category].[All]" allUniqueName="[Product].[Category].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product].[ID]" caption="ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Product].[ID].[All]" allUniqueName="[Product].[ID].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product].[Price]" caption="Price" attribute="1" defaultMemberUniqueName="[Product].[Price].[All]" allUniqueName="[Product].[Price].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product].[Special]" caption="Special" attribute="1" defaultMemberUniqueName="[Product].[Special].[All]" allUniqueName="[Product].[Special].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product].[Special-Category-Title]" caption="Special-Category-Title" defaultMemberUniqueName="[Product].[Special-Category-Title].[All]" allUniqueName="[Product].[Special-Category-Title].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product].[Title]" caption="Title" attribute="1" defaultMemberUniqueName="[Product].[Title].[All]" allUniqueName="[Product].[Title].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[Quantity]" caption="Quantity" measure="1" displayFolder="" measureGroup="Fact Order" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="4"/>
+        <fieldUsage x="1"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Net Amount]" caption="Net Amount" measure="1" displayFolder="" measureGroup="Fact Order" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="5"/>
+        <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Tax]" caption="Tax" measure="1" displayFolder="" measureGroup="Fact Order" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="6"/>
+        <fieldUsage x="2"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Total Amount]" caption="Total Amount" measure="1" displayFolder="" measureGroup="Fact Order" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="7"/>
+        <fieldUsage x="3"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Fact Order Count]" caption="Fact Order Count" measure="1" displayFolder="" measureGroup="Fact Order" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="8"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Fact Order Count]" caption="Fact Order Count" measure="1" displayFolder="" measureGroup="Fact Order" count="0"/>
   </cacheHierarchies>
   <kpis count="0"/>
   <dimensions count="5">
@@ -797,58 +618,14 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Oleg" refreshedDate="44172.583432060186" backgroundQuery="1" createdVersion="3" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D898D4B9-0A59-4E13-9679-63656F77784F}">
-  <cacheSource type="external" connectionId="1">
-    <extLst>
-      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
-        <x14:sourceConnection name="DS2 Cube"/>
-      </ext>
-    </extLst>
-  </cacheSource>
-  <cacheFields count="0"/>
-  <cacheHierarchies count="27">
-    <cacheHierarchy uniqueName="[Customer].[Age]" caption="Age" attribute="1" defaultMemberUniqueName="[Customer].[Age].[All]" allUniqueName="[Customer].[Age].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Customer ID]" caption="Customer ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Customer].[Customer ID].[All]" allUniqueName="[Customer].[Customer ID].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Full Name]" caption="Full Name" attribute="1" defaultMemberUniqueName="[Customer].[Full Name].[All]" allUniqueName="[Customer].[Full Name].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[Customer].[Gender].[All]" allUniqueName="[Customer].[Gender].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Customer].[Gender-Age-Name]" caption="Gender-Age-Name" defaultMemberUniqueName="[Customer].[Gender-Age-Name].[All]" allUniqueName="[Customer].[Gender-Age-Name].[All]" dimensionUniqueName="[Customer]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[Date ID]" caption="Date ID" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Date].[Date ID].[All]" allUniqueName="[Date].[Date ID].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[The Day]" caption="The Day" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Day].[All]" allUniqueName="[Date].[The Day].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[The Month]" caption="The Month" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Month].[All]" allUniqueName="[Date].[The Month].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[The Year]" caption="The Year" attribute="1" time="1" defaultMemberUniqueName="[Date].[The Year].[All]" allUniqueName="[Date].[The Year].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Date].[Year-Month-Day]" caption="Year-Month-Day" time="1" defaultMemberUniqueName="[Date].[Year-Month-Day].[All]" allUniqueName="[Date].[Year-Month-Day].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[City]" caption="City" attribute="1" defaultMemberUniqueName="[Location].[City].[All]" allUniqueName="[Location].[City].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Location].[Country].[All]" allUniqueName="[Location].[Country].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Location ID]" caption="Location ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Location].[Location ID].[All]" allUniqueName="[Location].[Location ID].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Region]" caption="Region" attribute="1" defaultMemberUniqueName="[Location].[Region].[All]" allUniqueName="[Location].[Region].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[Region-Country-State-City]" caption="Region-Country-State-City" defaultMemberUniqueName="[Location].[Region-Country-State-City].[All]" allUniqueName="[Location].[Region-Country-State-City].[All]" dimensionUniqueName="[Location]" displayFolder="" count="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Location].[State]" caption="State" attribute="1" defaultMemberUniqueName="[Location].[State].[All]" allUniqueName="[Location].[State].[All]" dimensionUniqueName="[Location]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Category]" caption="Category" attribute="1" defaultMemberUniqueName="[Product].[Category].[All]" allUniqueName="[Product].[Category].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[ID]" caption="ID" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Product].[ID].[All]" allUniqueName="[Product].[ID].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Price]" caption="Price" attribute="1" defaultMemberUniqueName="[Product].[Price].[All]" allUniqueName="[Product].[Price].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Special]" caption="Special" attribute="1" defaultMemberUniqueName="[Product].[Special].[All]" allUniqueName="[Product].[Special].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Special-Category-Title]" caption="Special-Category-Title" defaultMemberUniqueName="[Product].[Special-Category-Title].[All]" allUniqueName="[Product].[Special-Category-Title].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product].[Title]" caption="Title" attribute="1" defaultMemberUniqueName="[Product].[Title].[All]" allUniqueName="[Product].[Title].[All]" dimensionUniqueName="[Product]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Quantity]" caption="Quantity" measure="1" displayFolder="" measureGroup="Fact Order" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Net Amount]" caption="Net Amount" measure="1" displayFolder="" measureGroup="Fact Order" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Tax]" caption="Tax" measure="1" displayFolder="" measureGroup="Fact Order" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Total Amount]" caption="Total Amount" measure="1" displayFolder="" measureGroup="Fact Order" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fact Order Count]" caption="Fact Order Count" measure="1" displayFolder="" measureGroup="Fact Order" count="0"/>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition slicerData="1" pivotCacheId="2084384747" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D2D2F41-7E1D-4EB4-9424-E8A0E3D02548}" name="PivotTable1" cacheId="92" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A1:F4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D2B3BE42-41D2-4072-8618-E9FE99955DA9}" name="PivotTable1" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A1:E4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0">
       <items count="2">
         <item c="1" x="0"/>
@@ -858,14 +635,9 @@
     <pivotField axis="axisRow" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0"/>
     <pivotField axis="axisRow" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0"/>
     <pivotField axis="axisRow" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="0"/>
+    <field x="4"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -881,7 +653,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="5">
+  <colItems count="4">
     <i>
       <x/>
     </i>
@@ -894,16 +666,12 @@
     <i i="3">
       <x v="3"/>
     </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
   </colItems>
-  <dataFields count="5">
-    <dataField fld="4" baseField="0" baseItem="0"/>
-    <dataField fld="5" baseField="0" baseItem="0"/>
-    <dataField fld="6" baseField="0" baseItem="0"/>
-    <dataField fld="7" baseField="0" baseItem="0"/>
-    <dataField fld="8" baseField="0" baseItem="0"/>
+  <dataFields count="4">
+    <dataField fld="1" baseField="0" baseItem="0"/>
+    <dataField fld="0" baseField="0" baseItem="0"/>
+    <dataField fld="2" baseField="0" baseItem="0"/>
+    <dataField fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotHierarchies count="27">
     <pivotHierarchy/>
@@ -920,7 +688,7 @@
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
-    <pivotHierarchy multipleItemSelectionAllowed="1"/>
+    <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -953,7 +721,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{16AB70D4-E0AD-4FE3-A488-5AFE54EFBC32}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="3" xr16:uid="{16AB70D4-E0AD-4FE3-A488-5AFE54EFBC32}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
     <queryTableFields count="6">
       <queryTableField id="1" name="[Location].[Country].[Country].[MEMBER_CAPTION]" tableColumnId="7"/>
@@ -968,7 +736,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="3" xr16:uid="{6B15380E-4E77-447D-BD39-D6990A72077B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{6B15380E-4E77-447D-BD39-D6990A72077B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" name="[Measures].[Total Amount].[Location].[City].&amp;[Rqxsyse]" tableColumnId="2"/>
@@ -978,7 +746,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{FEEA925E-0C7A-48B0-A802-7E60FF4F6062}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="5" xr16:uid="{FEEA925E-0C7A-48B0-A802-7E60FF4F6062}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="9">
     <queryTableFields count="8">
       <queryTableField id="1" name="[Location].[Country].[Country].[MEMBER_CAPTION]" tableColumnId="9"/>
@@ -992,80 +760,6 @@
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
-</file>
-
-<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Region_Country_State_City" xr10:uid="{4A005CD5-2794-4888-82EA-1E8E421645D8}" sourceName="[Location].[Region-Country-State-City]">
-  <pivotTables>
-    <pivotTable tabId="1" name="PivotTable1"/>
-  </pivotTables>
-  <data>
-    <olap pivotCacheId="2084384747">
-      <levels count="5">
-        <level uniqueName="[Location].[Region-Country-State-City].[(All)]" sourceCaption="(All)" count="0"/>
-        <level uniqueName="[Location].[Region-Country-State-City].[Region]" sourceCaption="Region" count="2">
-          <ranges>
-            <range startItem="0">
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]" c="Non-USA"/>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[USA]" c="USA"/>
-            </range>
-          </ranges>
-        </level>
-        <level uniqueName="[Location].[Region-Country-State-City].[Country]" sourceCaption="Country" count="11">
-          <ranges>
-            <range startItem="0">
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[Australia]" c="Australia">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[Canada]" c="Canada">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[Chile]" c="Chile">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[China]" c="China">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[France]" c="France">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[Germany]" c="Germany">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[Japan]" c="Japan">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[Russia]" c="Russia">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[South Africa]" c="South Africa">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA].&amp;[UK]" c="UK">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[Non-USA]"/>
-              </i>
-              <i n="[Location].[Region-Country-State-City].[Region].&amp;[USA].&amp;[US]" c="US">
-                <p n="[Location].[Region-Country-State-City].[Region].&amp;[USA]"/>
-              </i>
-            </range>
-          </ranges>
-        </level>
-        <level uniqueName="[Location].[Region-Country-State-City].[State]" sourceCaption="State" count="0"/>
-        <level uniqueName="[Location].[Region-Country-State-City].[City]" sourceCaption="City" count="0"/>
-      </levels>
-      <selections count="1">
-        <selection n="[Location].[Region-Country-State-City].[All]"/>
-      </selections>
-    </olap>
-  </data>
-</slicerCacheDefinition>
-</file>
-
-<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Region" xr10:uid="{076845B5-CB69-4169-8E4B-160C1FD9BCE3}" cache="Slicer_Region_Country_State_City" caption="Region" level="1" rowHeight="241300"/>
-  <slicer name="Country" xr10:uid="{35516568-88C1-4A81-BCD2-281ADC07BFD0}" cache="Slicer_Region_Country_State_City" caption="Country" level="2" rowHeight="241300"/>
-</slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1406,11 +1100,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36490209-6DA8-4DC0-BE02-712F1A084E08}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B5D186-C634-458D-9EB4-DDDFC3DD8C3D}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,10 +1114,9 @@
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
@@ -1439,11 +1132,8 @@
       <c r="E1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>121</v>
       </c>
@@ -1451,19 +1141,16 @@
         <v>60951</v>
       </c>
       <c r="C2" s="1">
-        <v>1219296.5699995591</v>
+        <v>1219264.4900000188</v>
       </c>
       <c r="D2" s="1">
-        <v>100589.63999999857</v>
+        <v>100586.97999999838</v>
       </c>
       <c r="E2" s="1">
-        <v>1319886.2099999394</v>
-      </c>
-      <c r="F2" s="1">
-        <v>30460</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1319851.4699999932</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>122</v>
       </c>
@@ -1471,19 +1158,16 @@
         <v>59768</v>
       </c>
       <c r="C3" s="1">
-        <v>1192654.3299995705</v>
+        <v>1192650.3199995705</v>
       </c>
       <c r="D3" s="1">
-        <v>98391.919999998121</v>
+        <v>98391.57999999811</v>
       </c>
       <c r="E3" s="1">
-        <v>1291046.2499999485</v>
-      </c>
-      <c r="F3" s="1">
-        <v>29890</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1291041.8999999487</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>123</v>
       </c>
@@ -1491,28 +1175,17 @@
         <v>120719</v>
       </c>
       <c r="C4" s="1">
-        <v>2411950.8999999887</v>
+        <v>2411914.8100002208</v>
       </c>
       <c r="D4" s="1">
-        <v>198981.56000000038</v>
+        <v>198978.56000002605</v>
       </c>
       <c r="E4" s="1">
-        <v>2610932.4599999962</v>
-      </c>
-      <c r="F4" s="1">
-        <v>60350</v>
+        <v>2610893.3699996448</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
-      <x14:slicerList>
-        <x14:slicer r:id="rId3"/>
-      </x14:slicerList>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>